<commit_message>
replacing data storage for RDS format
</commit_message>
<xml_diff>
--- a/output/SZF6101VIP3_count-2022-06-28.xlsx
+++ b/output/SZF6101VIP3_count-2022-06-28.xlsx
@@ -402,7 +402,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>57</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>141</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">

</xml_diff>